<commit_message>
updated bee action function
</commit_message>
<xml_diff>
--- a/sprint 2 plan 19.4.2021.xlsx
+++ b/sprint 2 plan 19.4.2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Downloads/CSY026SE-AntsVsBees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F842ED9-1520-944A-8917-306D255D2041}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8602D8-8F24-C54A-81CE-619F182ABC98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Names</t>
   </si>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,7 +822,9 @@
       <c r="D12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -835,7 +837,9 @@
       <c r="D13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>

</xml_diff>

<commit_message>
Guide menu added guidemenu.docx needs to be updated
</commit_message>
<xml_diff>
--- a/sprint 2 plan 19.4.2021.xlsx
+++ b/sprint 2 plan 19.4.2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Downloads/CSY026SE-AntsVsBees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8602D8-8F24-C54A-81CE-619F182ABC98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E5C4C-1538-5747-BB6C-542E917F91B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Names</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Done with wallant branch. Separate branch not created</t>
   </si>
   <si>
-    <t>Create user accounts. Allow saving the level of a game for each user account</t>
-  </si>
-  <si>
     <t>Include a help/guide menu that shows the description of each ant and bee</t>
   </si>
   <si>
@@ -215,6 +212,24 @@
   </si>
   <si>
     <t>add_levels_to_game</t>
+  </si>
+  <si>
+    <t>Complete all black box tests</t>
+  </si>
+  <si>
+    <t>Slow thrower ant and its tests</t>
+  </si>
+  <si>
+    <t>Queen ants and its tests</t>
+  </si>
+  <si>
+    <t>Stun thrower and its test</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Add levels to the game</t>
   </si>
 </sst>
 </file>
@@ -261,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,8 +289,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -298,12 +319,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -321,6 +355,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -820,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>50</v>
@@ -835,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>50</v>
@@ -850,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -958,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="6"/>
     </row>
@@ -1091,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8814B48-8DC8-3F4F-9483-6736E797D3CE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1124,41 +1164,120 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="12">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/Muhammadali945/CSY026SE-AntsVsBees/tree/add_levels_to_game" xr:uid="{BD0B2193-2421-B440-997D-05EBF39A9AF6}"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/Muhammadali945/CSY026SE-AntsVsBees/tree/add_levels_to_game" xr:uid="{B2ED13FD-DF56-994F-B634-96CFBBC3E102}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>